<commit_message>
fixed excel last item including
</commit_message>
<xml_diff>
--- a/Books/il.xlsx
+++ b/Books/il.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\DalistoTask2\Books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA9C81C-E048-45F0-B2EA-A9C3E8803A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C7F6DE-562F-4D59-B1AA-AEB25EAA39B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>ADIYAMAN</t>
   </si>
   <si>
-    <t>AFYON</t>
-  </si>
-  <si>
     <t>AĞRI</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>ISPARTA</t>
   </si>
   <si>
-    <t>İÇEL</t>
-  </si>
-  <si>
     <t>İSTANBUL</t>
   </si>
   <si>
@@ -159,10 +153,6 @@
     <t>MALATYA</t>
   </si>
   <si>
-    <t xml:space="preserve">MANİSA_x000D_
-</t>
-  </si>
-  <si>
     <t>KAHRAMANMARAŞ</t>
   </si>
   <si>
@@ -265,10 +255,6 @@
     <t>KİLİS</t>
   </si>
   <si>
-    <t xml:space="preserve">OSMANİYE_x000D_
-</t>
-  </si>
-  <si>
     <t>DÜZCE</t>
   </si>
   <si>
@@ -276,6 +262,18 @@
   </si>
   <si>
     <t>CountryId</t>
+  </si>
+  <si>
+    <t>MANİSA</t>
+  </si>
+  <si>
+    <t>OSMANİYE</t>
+  </si>
+  <si>
+    <t>MERSİN</t>
+  </si>
+  <si>
+    <t>AFYONKARAHİSAR</t>
   </si>
 </sst>
 </file>
@@ -600,20 +598,21 @@
   <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B2" sqref="B2:B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -637,7 +636,7 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -645,7 +644,7 @@
         <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -653,7 +652,7 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -661,7 +660,7 @@
         <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -669,7 +668,7 @@
         <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -677,7 +676,7 @@
         <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -685,7 +684,7 @@
         <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -693,7 +692,7 @@
         <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -701,7 +700,7 @@
         <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -709,7 +708,7 @@
         <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -717,7 +716,7 @@
         <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -725,7 +724,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -733,7 +732,7 @@
         <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -741,7 +740,7 @@
         <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -749,7 +748,7 @@
         <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -757,7 +756,7 @@
         <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -765,7 +764,7 @@
         <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -773,7 +772,7 @@
         <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -781,7 +780,7 @@
         <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -789,7 +788,7 @@
         <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -797,7 +796,7 @@
         <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -805,7 +804,7 @@
         <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -813,7 +812,7 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -821,7 +820,7 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -829,7 +828,7 @@
         <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -837,7 +836,7 @@
         <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -845,7 +844,7 @@
         <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -853,7 +852,7 @@
         <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -861,7 +860,7 @@
         <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -869,7 +868,7 @@
         <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -877,7 +876,7 @@
         <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -885,7 +884,7 @@
         <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -893,7 +892,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -901,7 +900,7 @@
         <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -909,7 +908,7 @@
         <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -917,7 +916,7 @@
         <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -925,7 +924,7 @@
         <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -933,7 +932,7 @@
         <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -941,7 +940,7 @@
         <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -949,7 +948,7 @@
         <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -957,7 +956,7 @@
         <v>70</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -965,15 +964,15 @@
         <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>70</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -981,7 +980,7 @@
         <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -989,7 +988,7 @@
         <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -997,7 +996,7 @@
         <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1005,7 +1004,7 @@
         <v>70</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1013,7 +1012,7 @@
         <v>70</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1021,7 +1020,7 @@
         <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1029,7 +1028,7 @@
         <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1037,7 +1036,7 @@
         <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1045,7 +1044,7 @@
         <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1053,7 +1052,7 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1061,7 +1060,7 @@
         <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1069,7 +1068,7 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1077,7 +1076,7 @@
         <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1085,7 +1084,7 @@
         <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1093,7 +1092,7 @@
         <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1101,7 +1100,7 @@
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1109,7 +1108,7 @@
         <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1117,7 +1116,7 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1125,7 +1124,7 @@
         <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1133,7 +1132,7 @@
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1141,7 +1140,7 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1149,7 +1148,7 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1157,7 +1156,7 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1165,7 +1164,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1173,7 +1172,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1181,7 +1180,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1189,7 +1188,7 @@
         <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1197,7 +1196,7 @@
         <v>70</v>
       </c>
       <c r="B74" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1205,7 +1204,7 @@
         <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1213,7 +1212,7 @@
         <v>70</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1221,7 +1220,7 @@
         <v>70</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1229,7 +1228,7 @@
         <v>70</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1237,7 +1236,7 @@
         <v>70</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1245,15 +1244,15 @@
         <v>70</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>70</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1261,7 +1260,7 @@
         <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>